<commit_message>
Ajout des taux d'accroissement
</commit_message>
<xml_diff>
--- a/donnees_enrichies.xlsx
+++ b/donnees_enrichies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,16 @@
           <t>Ratio Jeunes</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Taux accroiss Population</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Taux accroiss PIB</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -556,6 +566,8 @@
       <c r="O2" t="n">
         <v>39.92026209961882</v>
       </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -603,6 +615,12 @@
       <c r="O3" t="n">
         <v>40.33541683315063</v>
       </c>
+      <c r="P3" t="n">
+        <v>1.852411390512154</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>9.970958099789119</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -650,6 +668,12 @@
       <c r="O4" t="n">
         <v>40.76800210650654</v>
       </c>
+      <c r="P4" t="n">
+        <v>1.925999695428571</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5.181413503482668</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -697,6 +721,12 @@
       <c r="O5" t="n">
         <v>41.21667435357455</v>
       </c>
+      <c r="P5" t="n">
+        <v>1.994561396566508</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2.987860694167144</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -744,6 +774,12 @@
       <c r="O6" t="n">
         <v>41.64788472656066</v>
       </c>
+      <c r="P6" t="n">
+        <v>2.044318649888899</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.916501943455562</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -791,6 +827,12 @@
       <c r="O7" t="n">
         <v>42.06236553675482</v>
       </c>
+      <c r="P7" t="n">
+        <v>2.085052963116807</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.5354274781566137</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -838,6 +880,12 @@
       <c r="O8" t="n">
         <v>42.45580738156201</v>
       </c>
+      <c r="P8" t="n">
+        <v>2.132268150645489</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.8792861413132735</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -885,6 +933,12 @@
       <c r="O9" t="n">
         <v>42.82999343777855</v>
       </c>
+      <c r="P9" t="n">
+        <v>2.17993856707166</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0253902930783978</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -932,6 +986,12 @@
       <c r="O10" t="n">
         <v>43.18365041824671</v>
       </c>
+      <c r="P10" t="n">
+        <v>2.229154478887807</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-0.06933550214139883</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -979,6 +1039,12 @@
       <c r="O11" t="n">
         <v>43.51435744895195</v>
       </c>
+      <c r="P11" t="n">
+        <v>2.274345958329649</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-0.8466397374539025</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1026,6 +1092,12 @@
       <c r="O12" t="n">
         <v>43.81937261938072</v>
       </c>
+      <c r="P12" t="n">
+        <v>2.321576053339869</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>6.554044594604358</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1073,6 +1145,12 @@
       <c r="O13" t="n">
         <v>44.09356673496786</v>
       </c>
+      <c r="P13" t="n">
+        <v>2.367949548922654</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.1756615742589895</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1120,6 +1198,12 @@
       <c r="O14" t="n">
         <v>44.33503448042055</v>
       </c>
+      <c r="P14" t="n">
+        <v>2.410144553244464</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-9.631429332847564</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1167,6 +1251,12 @@
       <c r="O15" t="n">
         <v>44.5458693269039</v>
       </c>
+      <c r="P15" t="n">
+        <v>2.461582932184392</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1.527658133522558</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1214,6 +1304,12 @@
       <c r="O16" t="n">
         <v>44.71544047952038</v>
       </c>
+      <c r="P16" t="n">
+        <v>2.518976713055965</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.948080621982795</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1261,6 +1357,12 @@
       <c r="O17" t="n">
         <v>44.8477755311462</v>
       </c>
+      <c r="P17" t="n">
+        <v>2.576470841368939</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>2.904257369893015</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1308,6 +1410,12 @@
       <c r="O18" t="n">
         <v>44.95786991086932</v>
       </c>
+      <c r="P18" t="n">
+        <v>2.624832951626765</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.291492466254617</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1355,6 +1463,12 @@
       <c r="O19" t="n">
         <v>45.06416542393228</v>
       </c>
+      <c r="P19" t="n">
+        <v>2.695394810269724</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1.801502139996458</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1402,6 +1516,12 @@
       <c r="O20" t="n">
         <v>45.396218489649</v>
       </c>
+      <c r="P20" t="n">
+        <v>3.196780246327857</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-0.7361991832215198</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1449,6 +1569,12 @@
       <c r="O21" t="n">
         <v>45.52264966453907</v>
       </c>
+      <c r="P21" t="n">
+        <v>2.899917692680876</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-0.5763285310710353</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1496,6 +1622,12 @@
       <c r="O22" t="n">
         <v>45.63129602363561</v>
       </c>
+      <c r="P22" t="n">
+        <v>2.938482432553169</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-0.5749280374805377</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1543,6 +1675,12 @@
       <c r="O23" t="n">
         <v>45.72271467056205</v>
       </c>
+      <c r="P23" t="n">
+        <v>2.973254918159052</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-0.5548149536395264</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1590,6 +1728,12 @@
       <c r="O24" t="n">
         <v>45.79751031918469</v>
       </c>
+      <c r="P24" t="n">
+        <v>3.0043796952264</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>-0.517752003162586</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1637,6 +1781,12 @@
       <c r="O25" t="n">
         <v>45.85632498309322</v>
       </c>
+      <c r="P25" t="n">
+        <v>3.032007665413428</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>-0.4654866066174934</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1684,6 +1834,12 @@
       <c r="O26" t="n">
         <v>45.8998285347611</v>
       </c>
+      <c r="P26" t="n">
+        <v>3.056294153665351</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>-0.3997566988461876</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1731,6 +1887,12 @@
       <c r="O27" t="n">
         <v>45.92871016114523</v>
       </c>
+      <c r="P27" t="n">
+        <v>3.077397191895126</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-0.3222906799551839</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1778,6 +1940,12 @@
       <c r="O28" t="n">
         <v>45.94367072162582</v>
       </c>
+      <c r="P28" t="n">
+        <v>3.095475957045557</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>-0.2348019334505569</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1825,6 +1993,12 @@
       <c r="O29" t="n">
         <v>45.94541598924614</v>
       </c>
+      <c r="P29" t="n">
+        <v>3.110689418905555</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>-0.1389793034266895</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1872,6 +2046,12 @@
       <c r="O30" t="n">
         <v>45.93465074443909</v>
       </c>
+      <c r="P30" t="n">
+        <v>3.123195172000659</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>-0.03647453289306046</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1919,6 +2099,12 @@
       <c r="O31" t="n">
         <v>45.91207367888527</v>
       </c>
+      <c r="P31" t="n">
+        <v>3.133148425993437</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.07111228798437619</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1966,6 +2152,12 @@
       <c r="O32" t="n">
         <v>45.87837305856756</v>
       </c>
+      <c r="P32" t="n">
+        <v>3.140701160893289</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.182248232355664</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2013,6 +2205,12 @@
       <c r="O33" t="n">
         <v>45.83422308721779</v>
       </c>
+      <c r="P33" t="n">
+        <v>3.146001437827861</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.2954826183072301</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2060,6 +2258,12 @@
       <c r="O34" t="n">
         <v>45.78028091152648</v>
       </c>
+      <c r="P34" t="n">
+        <v>3.149192836566606</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.4094615340172858</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2107,6 +2311,12 @@
       <c r="O35" t="n">
         <v>45.71718420994092</v>
       </c>
+      <c r="P35" t="n">
+        <v>3.150414015172776</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.522940078818146</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2154,6 +2364,12 @@
       <c r="O36" t="n">
         <v>45.64554929829949</v>
       </c>
+      <c r="P36" t="n">
+        <v>3.149798380391999</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.6347923891886653</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2201,6 +2417,12 @@
       <c r="O37" t="n">
         <v>45.56596970315129</v>
       </c>
+      <c r="P37" t="n">
+        <v>3.147473847524251</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.7440189310775391</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2248,6 +2470,12 @@
       <c r="O38" t="n">
         <v>45.47901513681313</v>
       </c>
+      <c r="P38" t="n">
+        <v>3.143562697162627</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.8497505936860605</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2295,6 +2523,12 @@
       <c r="O39" t="n">
         <v>45.60556193235352</v>
       </c>
+      <c r="P39" t="n">
+        <v>2.906151181259209</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>3.733039025005702</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2342,6 +2576,12 @@
       <c r="O40" t="n">
         <v>45.43837746078823</v>
       </c>
+      <c r="P40" t="n">
+        <v>3.12447074877571</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>2.838707853544364</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2389,6 +2629,12 @@
       <c r="O41" t="n">
         <v>45.2626962300936</v>
       </c>
+      <c r="P41" t="n">
+        <v>3.101479045072852</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>1.999548844771426</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2436,6 +2682,12 @@
       <c r="O42" t="n">
         <v>45.08483013940658</v>
       </c>
+      <c r="P42" t="n">
+        <v>3.086791171586545</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>1.51752867785675</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2483,6 +2735,12 @@
       <c r="O43" t="n">
         <v>44.91369342113743</v>
       </c>
+      <c r="P43" t="n">
+        <v>3.096166909823639</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.3497930373576263</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2530,6 +2788,12 @@
       <c r="O44" t="n">
         <v>44.76014738891352</v>
       </c>
+      <c r="P44" t="n">
+        <v>3.109084084937952</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>1.382537855867638</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2577,6 +2841,12 @@
       <c r="O45" t="n">
         <v>44.57127985062206</v>
       </c>
+      <c r="P45" t="n">
+        <v>3.273034971775046</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>-1.621780028301745</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2624,6 +2894,12 @@
       <c r="O46" t="n">
         <v>44.43841549562293</v>
       </c>
+      <c r="P46" t="n">
+        <v>3.169872245240524</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.8481851881178004</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2671,6 +2947,12 @@
       <c r="O47" t="n">
         <v>44.3714904530047</v>
       </c>
+      <c r="P47" t="n">
+        <v>2.99919178598731</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>2.959561487677131</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2718,6 +3000,12 @@
       <c r="O48" t="n">
         <v>44.26045997243746</v>
       </c>
+      <c r="P48" t="n">
+        <v>3.065646083876339</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>1.768132925069521</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2765,6 +3053,12 @@
       <c r="O49" t="n">
         <v>44.0858819720187</v>
       </c>
+      <c r="P49" t="n">
+        <v>3.04446047696334</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>-0.6932574407960579</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2812,6 +3106,12 @@
       <c r="O50" t="n">
         <v>43.89894895464999</v>
       </c>
+      <c r="P50" t="n">
+        <v>3.029216388838729</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>-0.9142356841476795</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2859,6 +3159,12 @@
       <c r="O51" t="n">
         <v>43.76269830155642</v>
       </c>
+      <c r="P51" t="n">
+        <v>3.022602537549424</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-0.04719822755828718</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2906,6 +3212,12 @@
       <c r="O52" t="n">
         <v>43.65478203406788</v>
       </c>
+      <c r="P52" t="n">
+        <v>3.012139446856699</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>1.631847815600751</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2953,6 +3265,12 @@
       <c r="O53" t="n">
         <v>43.5668506751926</v>
       </c>
+      <c r="P53" t="n">
+        <v>2.992760772931846</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>4.125162298328844</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3000,6 +3318,12 @@
       <c r="O54" t="n">
         <v>43.48267885862412</v>
       </c>
+      <c r="P54" t="n">
+        <v>2.999112695182315</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>3.331830131562641</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3047,6 +3371,12 @@
       <c r="O55" t="n">
         <v>43.39789137640604</v>
       </c>
+      <c r="P55" t="n">
+        <v>2.997977153952069</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>-1.297448523688027</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3094,6 +3424,12 @@
       <c r="O56" t="n">
         <v>43.3119392154527</v>
       </c>
+      <c r="P56" t="n">
+        <v>2.967788638726843</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.4367820263125211</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3141,6 +3477,12 @@
       <c r="O57" t="n">
         <v>43.20801542885335</v>
       </c>
+      <c r="P57" t="n">
+        <v>2.923086155549037</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>2.604237999880965</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3188,6 +3530,12 @@
       <c r="O58" t="n">
         <v>43.06539891576168</v>
       </c>
+      <c r="P58" t="n">
+        <v>2.853598653795997</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>3.707277200582371</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3235,6 +3583,12 @@
       <c r="O59" t="n">
         <v>42.87698238867645</v>
       </c>
+      <c r="P59" t="n">
+        <v>2.773143642021814</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>4.003586262137659</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3282,6 +3636,12 @@
       <c r="O60" t="n">
         <v>42.6531783942503</v>
       </c>
+      <c r="P60" t="n">
+        <v>2.698362622679551</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>1.207015223707297</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3329,6 +3689,12 @@
       <c r="O61" t="n">
         <v>42.39886451006481</v>
       </c>
+      <c r="P61" t="n">
+        <v>2.626194045386865</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>4.377109446420091</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3376,6 +3742,12 @@
       <c r="O62" t="n">
         <v>42.1206314865863</v>
       </c>
+      <c r="P62" t="n">
+        <v>2.580133011595787</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>3.5449095030474</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -3422,6 +3794,12 @@
       </c>
       <c r="O63" t="n">
         <v>41.83626650476972</v>
+      </c>
+      <c r="P63" t="n">
+        <v>2.55483828955716</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>3.31407470119367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>